<commit_message>
Changed labelling and dates for the 18-21 mos dataset from 21 mos to 18 mos
</commit_message>
<xml_diff>
--- a/raw/training_validation_2_alldata.xlsx
+++ b/raw/training_validation_2_alldata.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unsw-my.sharepoint.com/personal/z5204897_ad_unsw_edu_au1/Documents/Desktop/WRL/R/raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2146" documentId="8_{0E982C34-0F34-499A-9533-E44D6D9B9A02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D1B7FBF4-175E-4294-82FF-9F05A276C54D}"/>
+  <xr:revisionPtr revIDLastSave="2155" documentId="8_{0E982C34-0F34-499A-9533-E44D6D9B9A02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6FD62348-4EEA-4588-9E30-84BE795D8F93}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{18870795-2872-4EB1-9916-EEEDE2D09B51}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="7" xr2:uid="{18870795-2872-4EB1-9916-EEEDE2D09B51}"/>
   </bookViews>
   <sheets>
     <sheet name="0mos" sheetId="1" r:id="rId1"/>
     <sheet name="9mos" sheetId="2" r:id="rId2"/>
-    <sheet name="21mos" sheetId="3" r:id="rId3"/>
+    <sheet name="18mos" sheetId="3" r:id="rId3"/>
     <sheet name="26mos" sheetId="4" r:id="rId4"/>
     <sheet name="34mos" sheetId="5" r:id="rId5"/>
     <sheet name="42mos" sheetId="6" r:id="rId6"/>
@@ -776,9 +776,6 @@
     <t>sarc_clump</t>
   </si>
   <si>
-    <t>21mos</t>
-  </si>
-  <si>
     <t>26mos</t>
   </si>
   <si>
@@ -795,6 +792,9 @@
   </si>
   <si>
     <t>Producers</t>
+  </si>
+  <si>
+    <t>18mos</t>
   </si>
 </sst>
 </file>
@@ -1174,7 +1174,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96B909E0-4A0E-4849-AEE5-CE255B2B44F0}">
   <dimension ref="B1:N65"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="O17" sqref="O17"/>
     </sheetView>
   </sheetViews>
@@ -12499,8 +12499,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D89CA01-BD8C-4745-BE15-7BAAE8E321D1}">
   <dimension ref="A1:F225"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K216" sqref="K216"/>
+    <sheetView tabSelected="1" topLeftCell="A60" workbookViewId="0">
+      <selection activeCell="J83" sqref="J83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -12524,10 +12524,10 @@
         <v>232</v>
       </c>
       <c r="E1" t="s">
+        <v>241</v>
+      </c>
+      <c r="F1" t="s">
         <v>242</v>
-      </c>
-      <c r="F1" t="s">
-        <v>243</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
@@ -13732,10 +13732,10 @@
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>237</v>
+        <v>243</v>
       </c>
       <c r="B62" s="4">
-        <v>43413</v>
+        <v>43334</v>
       </c>
       <c r="C62">
         <v>1</v>
@@ -13752,10 +13752,10 @@
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>237</v>
+        <v>243</v>
       </c>
       <c r="B63" s="4">
-        <v>43413</v>
+        <v>43334</v>
       </c>
       <c r="C63">
         <v>1</v>
@@ -13772,10 +13772,10 @@
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>237</v>
+        <v>243</v>
       </c>
       <c r="B64" s="4">
-        <v>43413</v>
+        <v>43334</v>
       </c>
       <c r="C64">
         <v>1</v>
@@ -13792,10 +13792,10 @@
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>237</v>
+        <v>243</v>
       </c>
       <c r="B65" s="4">
-        <v>43413</v>
+        <v>43334</v>
       </c>
       <c r="C65">
         <v>1</v>
@@ -13812,10 +13812,10 @@
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>237</v>
+        <v>243</v>
       </c>
       <c r="B66" s="4">
-        <v>43413</v>
+        <v>43334</v>
       </c>
       <c r="C66">
         <v>1</v>
@@ -13832,10 +13832,10 @@
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>237</v>
+        <v>243</v>
       </c>
       <c r="B67" s="4">
-        <v>43413</v>
+        <v>43334</v>
       </c>
       <c r="C67">
         <v>1</v>
@@ -13852,10 +13852,10 @@
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>237</v>
+        <v>243</v>
       </c>
       <c r="B68" s="4">
-        <v>43413</v>
+        <v>43334</v>
       </c>
       <c r="C68">
         <v>1</v>
@@ -13872,10 +13872,10 @@
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>237</v>
+        <v>243</v>
       </c>
       <c r="B69" s="4">
-        <v>43413</v>
+        <v>43334</v>
       </c>
       <c r="C69">
         <v>1</v>
@@ -13892,10 +13892,10 @@
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>237</v>
+        <v>243</v>
       </c>
       <c r="B70" s="4">
-        <v>43413</v>
+        <v>43334</v>
       </c>
       <c r="C70">
         <v>2</v>
@@ -13912,10 +13912,10 @@
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>237</v>
+        <v>243</v>
       </c>
       <c r="B71" s="4">
-        <v>43413</v>
+        <v>43334</v>
       </c>
       <c r="C71">
         <v>2</v>
@@ -13932,10 +13932,10 @@
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>237</v>
+        <v>243</v>
       </c>
       <c r="B72" s="4">
-        <v>43413</v>
+        <v>43334</v>
       </c>
       <c r="C72">
         <v>2</v>
@@ -13952,10 +13952,10 @@
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>237</v>
+        <v>243</v>
       </c>
       <c r="B73" s="4">
-        <v>43413</v>
+        <v>43334</v>
       </c>
       <c r="C73">
         <v>2</v>
@@ -13972,10 +13972,10 @@
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>237</v>
+        <v>243</v>
       </c>
       <c r="B74" s="4">
-        <v>43413</v>
+        <v>43334</v>
       </c>
       <c r="C74">
         <v>2</v>
@@ -13992,10 +13992,10 @@
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>237</v>
+        <v>243</v>
       </c>
       <c r="B75" s="4">
-        <v>43413</v>
+        <v>43334</v>
       </c>
       <c r="C75">
         <v>2</v>
@@ -14012,10 +14012,10 @@
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>237</v>
+        <v>243</v>
       </c>
       <c r="B76" s="4">
-        <v>43413</v>
+        <v>43334</v>
       </c>
       <c r="C76">
         <v>2</v>
@@ -14032,10 +14032,10 @@
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>237</v>
+        <v>243</v>
       </c>
       <c r="B77" s="4">
-        <v>43413</v>
+        <v>43334</v>
       </c>
       <c r="C77">
         <v>2</v>
@@ -14052,10 +14052,10 @@
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>237</v>
+        <v>243</v>
       </c>
       <c r="B78" s="4">
-        <v>43413</v>
+        <v>43334</v>
       </c>
       <c r="C78">
         <v>0.1</v>
@@ -14072,10 +14072,10 @@
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>237</v>
+        <v>243</v>
       </c>
       <c r="B79" s="4">
-        <v>43413</v>
+        <v>43334</v>
       </c>
       <c r="C79">
         <v>0.1</v>
@@ -14092,10 +14092,10 @@
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>237</v>
+        <v>243</v>
       </c>
       <c r="B80" s="4">
-        <v>43413</v>
+        <v>43334</v>
       </c>
       <c r="C80">
         <v>0.1</v>
@@ -14112,10 +14112,10 @@
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
-        <v>237</v>
+        <v>243</v>
       </c>
       <c r="B81" s="4">
-        <v>43413</v>
+        <v>43334</v>
       </c>
       <c r="C81">
         <v>0.1</v>
@@ -14132,10 +14132,10 @@
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
-        <v>237</v>
+        <v>243</v>
       </c>
       <c r="B82" s="4">
-        <v>43413</v>
+        <v>43334</v>
       </c>
       <c r="C82">
         <v>0.1</v>
@@ -14152,10 +14152,10 @@
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
-        <v>237</v>
+        <v>243</v>
       </c>
       <c r="B83" s="4">
-        <v>43413</v>
+        <v>43334</v>
       </c>
       <c r="C83">
         <v>0.1</v>
@@ -14172,10 +14172,10 @@
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
-        <v>237</v>
+        <v>243</v>
       </c>
       <c r="B84" s="4">
-        <v>43413</v>
+        <v>43334</v>
       </c>
       <c r="C84">
         <v>0.1</v>
@@ -14192,10 +14192,10 @@
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
-        <v>237</v>
+        <v>243</v>
       </c>
       <c r="B85" s="4">
-        <v>43413</v>
+        <v>43334</v>
       </c>
       <c r="C85">
         <v>0.1</v>
@@ -14212,10 +14212,10 @@
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
-        <v>237</v>
+        <v>243</v>
       </c>
       <c r="B86" s="4">
-        <v>43414</v>
+        <v>43334</v>
       </c>
       <c r="C86">
         <v>0.5</v>
@@ -14232,10 +14232,10 @@
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
-        <v>237</v>
+        <v>243</v>
       </c>
       <c r="B87" s="4">
-        <v>43415</v>
+        <v>43334</v>
       </c>
       <c r="C87">
         <v>0.5</v>
@@ -14252,10 +14252,10 @@
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
-        <v>237</v>
+        <v>243</v>
       </c>
       <c r="B88" s="4">
-        <v>43416</v>
+        <v>43334</v>
       </c>
       <c r="C88">
         <v>0.5</v>
@@ -14272,10 +14272,10 @@
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
-        <v>237</v>
+        <v>243</v>
       </c>
       <c r="B89" s="4">
-        <v>43417</v>
+        <v>43334</v>
       </c>
       <c r="C89">
         <v>0.5</v>
@@ -14292,10 +14292,10 @@
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
-        <v>237</v>
+        <v>243</v>
       </c>
       <c r="B90" s="4">
-        <v>43418</v>
+        <v>43334</v>
       </c>
       <c r="C90">
         <v>0.5</v>
@@ -14312,10 +14312,10 @@
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
-        <v>237</v>
+        <v>243</v>
       </c>
       <c r="B91" s="4">
-        <v>43419</v>
+        <v>43334</v>
       </c>
       <c r="C91">
         <v>0.5</v>
@@ -14332,10 +14332,10 @@
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
-        <v>237</v>
+        <v>243</v>
       </c>
       <c r="B92" s="4">
-        <v>43420</v>
+        <v>43334</v>
       </c>
       <c r="C92">
         <v>0.5</v>
@@ -14352,10 +14352,10 @@
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
-        <v>237</v>
+        <v>243</v>
       </c>
       <c r="B93" s="4">
-        <v>43421</v>
+        <v>43334</v>
       </c>
       <c r="C93">
         <v>0.5</v>
@@ -14372,7 +14372,7 @@
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B94" s="4">
         <v>43585</v>
@@ -14392,7 +14392,7 @@
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B95" s="4">
         <v>43585</v>
@@ -14412,7 +14412,7 @@
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B96" s="4">
         <v>43585</v>
@@ -14432,7 +14432,7 @@
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B97" s="4">
         <v>43585</v>
@@ -14452,7 +14452,7 @@
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B98" s="4">
         <v>43585</v>
@@ -14472,7 +14472,7 @@
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B99" s="4">
         <v>43585</v>
@@ -14492,7 +14492,7 @@
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B100" s="4">
         <v>43585</v>
@@ -14512,7 +14512,7 @@
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B101" s="4">
         <v>43585</v>
@@ -14532,7 +14532,7 @@
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B102" s="4">
         <v>43585</v>
@@ -14552,7 +14552,7 @@
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B103" s="4">
         <v>43585</v>
@@ -14572,7 +14572,7 @@
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B104" s="4">
         <v>43585</v>
@@ -14592,7 +14592,7 @@
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B105" s="4">
         <v>43585</v>
@@ -14612,7 +14612,7 @@
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B106" s="4">
         <v>43585</v>
@@ -14632,7 +14632,7 @@
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B107" s="4">
         <v>43585</v>
@@ -14652,7 +14652,7 @@
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B108" s="4">
         <v>43585</v>
@@ -14672,7 +14672,7 @@
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B109" s="4">
         <v>43585</v>
@@ -14692,7 +14692,7 @@
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B110" s="4">
         <v>43585</v>
@@ -14712,7 +14712,7 @@
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B111" s="4">
         <v>43585</v>
@@ -14732,7 +14732,7 @@
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B112" s="4">
         <v>43585</v>
@@ -14752,7 +14752,7 @@
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B113" s="4">
         <v>43585</v>
@@ -14772,7 +14772,7 @@
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B114" s="4">
         <v>43585</v>
@@ -14792,7 +14792,7 @@
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B115" s="4">
         <v>43585</v>
@@ -14812,7 +14812,7 @@
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B116" s="4">
         <v>43585</v>
@@ -14832,7 +14832,7 @@
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B117" s="4">
         <v>43585</v>
@@ -14852,7 +14852,7 @@
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B118" s="4">
         <v>43585</v>
@@ -14872,7 +14872,7 @@
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B119" s="4">
         <v>43585</v>
@@ -14892,7 +14892,7 @@
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B120" s="4">
         <v>43585</v>
@@ -14912,7 +14912,7 @@
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B121" s="4">
         <v>43585</v>
@@ -14932,7 +14932,7 @@
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B122" s="4">
         <v>43585</v>
@@ -14952,7 +14952,7 @@
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B123" s="4">
         <v>43585</v>
@@ -14972,7 +14972,7 @@
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B124" s="4">
         <v>43585</v>
@@ -14992,7 +14992,7 @@
     </row>
     <row r="125" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B125" s="4">
         <v>43585</v>
@@ -15012,7 +15012,7 @@
     </row>
     <row r="126" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B126" s="4">
         <v>43817</v>
@@ -15032,7 +15032,7 @@
     </row>
     <row r="127" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B127" s="4">
         <v>43817</v>
@@ -15052,7 +15052,7 @@
     </row>
     <row r="128" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B128" s="4">
         <v>43817</v>
@@ -15072,7 +15072,7 @@
     </row>
     <row r="129" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B129" s="4">
         <v>43817</v>
@@ -15092,7 +15092,7 @@
     </row>
     <row r="130" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B130" s="4">
         <v>43817</v>
@@ -15112,7 +15112,7 @@
     </row>
     <row r="131" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B131" s="4">
         <v>43817</v>
@@ -15132,7 +15132,7 @@
     </row>
     <row r="132" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B132" s="4">
         <v>43817</v>
@@ -15152,7 +15152,7 @@
     </row>
     <row r="133" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B133" s="4">
         <v>43817</v>
@@ -15172,7 +15172,7 @@
     </row>
     <row r="134" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B134" s="4">
         <v>43817</v>
@@ -15192,7 +15192,7 @@
     </row>
     <row r="135" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B135" s="4">
         <v>43817</v>
@@ -15212,7 +15212,7 @@
     </row>
     <row r="136" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B136" s="4">
         <v>43817</v>
@@ -15232,7 +15232,7 @@
     </row>
     <row r="137" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B137" s="4">
         <v>43817</v>
@@ -15252,7 +15252,7 @@
     </row>
     <row r="138" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B138" s="4">
         <v>43817</v>
@@ -15272,7 +15272,7 @@
     </row>
     <row r="139" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B139" s="4">
         <v>43817</v>
@@ -15292,7 +15292,7 @@
     </row>
     <row r="140" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B140" s="4">
         <v>43817</v>
@@ -15312,7 +15312,7 @@
     </row>
     <row r="141" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B141" s="4">
         <v>43817</v>
@@ -15332,7 +15332,7 @@
     </row>
     <row r="142" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B142" s="4">
         <v>43817</v>
@@ -15352,7 +15352,7 @@
     </row>
     <row r="143" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B143" s="4">
         <v>43817</v>
@@ -15372,7 +15372,7 @@
     </row>
     <row r="144" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B144" s="4">
         <v>43817</v>
@@ -15392,7 +15392,7 @@
     </row>
     <row r="145" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B145" s="4">
         <v>43817</v>
@@ -15412,7 +15412,7 @@
     </row>
     <row r="146" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B146" s="4">
         <v>43817</v>
@@ -15432,7 +15432,7 @@
     </row>
     <row r="147" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B147" s="4">
         <v>43817</v>
@@ -15452,7 +15452,7 @@
     </row>
     <row r="148" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B148" s="4">
         <v>43817</v>
@@ -15472,7 +15472,7 @@
     </row>
     <row r="149" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B149" s="4">
         <v>43817</v>
@@ -15492,7 +15492,7 @@
     </row>
     <row r="150" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B150" s="4">
         <v>43817</v>
@@ -15512,7 +15512,7 @@
     </row>
     <row r="151" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B151" s="4">
         <v>43817</v>
@@ -15532,7 +15532,7 @@
     </row>
     <row r="152" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B152" s="4">
         <v>43817</v>
@@ -15552,7 +15552,7 @@
     </row>
     <row r="153" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B153" s="4">
         <v>43817</v>
@@ -15572,7 +15572,7 @@
     </row>
     <row r="154" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B154" s="4">
         <v>43817</v>
@@ -15592,7 +15592,7 @@
     </row>
     <row r="155" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B155" s="4">
         <v>43817</v>
@@ -15612,7 +15612,7 @@
     </row>
     <row r="156" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B156" s="4">
         <v>43817</v>
@@ -15632,7 +15632,7 @@
     </row>
     <row r="157" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A157" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B157" s="4">
         <v>43817</v>
@@ -15652,7 +15652,7 @@
     </row>
     <row r="158" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A158" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B158" s="4">
         <v>44056</v>
@@ -15672,7 +15672,7 @@
     </row>
     <row r="159" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A159" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B159" s="4">
         <v>44056</v>
@@ -15692,7 +15692,7 @@
     </row>
     <row r="160" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A160" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B160" s="4">
         <v>44056</v>
@@ -15712,7 +15712,7 @@
     </row>
     <row r="161" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A161" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B161" s="4">
         <v>44056</v>
@@ -15732,7 +15732,7 @@
     </row>
     <row r="162" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A162" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B162" s="4">
         <v>44056</v>
@@ -15752,7 +15752,7 @@
     </row>
     <row r="163" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A163" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B163" s="4">
         <v>44056</v>
@@ -15772,7 +15772,7 @@
     </row>
     <row r="164" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A164" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B164" s="4">
         <v>44056</v>
@@ -15792,7 +15792,7 @@
     </row>
     <row r="165" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A165" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B165" s="4">
         <v>44056</v>
@@ -15812,7 +15812,7 @@
     </row>
     <row r="166" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A166" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B166" s="4">
         <v>44056</v>
@@ -15832,7 +15832,7 @@
     </row>
     <row r="167" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A167" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B167" s="4">
         <v>44056</v>
@@ -15852,7 +15852,7 @@
     </row>
     <row r="168" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A168" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B168" s="4">
         <v>44056</v>
@@ -15872,7 +15872,7 @@
     </row>
     <row r="169" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A169" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B169" s="4">
         <v>44056</v>
@@ -15892,7 +15892,7 @@
     </row>
     <row r="170" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A170" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B170" s="4">
         <v>44056</v>
@@ -15912,7 +15912,7 @@
     </row>
     <row r="171" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A171" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B171" s="4">
         <v>44056</v>
@@ -15932,7 +15932,7 @@
     </row>
     <row r="172" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A172" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B172" s="4">
         <v>44056</v>
@@ -15952,7 +15952,7 @@
     </row>
     <row r="173" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A173" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B173" s="4">
         <v>44056</v>
@@ -15972,7 +15972,7 @@
     </row>
     <row r="174" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A174" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B174" s="4">
         <v>44056</v>
@@ -15992,7 +15992,7 @@
     </row>
     <row r="175" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A175" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B175" s="4">
         <v>44056</v>
@@ -16012,7 +16012,7 @@
     </row>
     <row r="176" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A176" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B176" s="4">
         <v>44056</v>
@@ -16032,7 +16032,7 @@
     </row>
     <row r="177" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A177" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B177" s="4">
         <v>44056</v>
@@ -16052,7 +16052,7 @@
     </row>
     <row r="178" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A178" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B178" s="4">
         <v>44056</v>
@@ -16072,7 +16072,7 @@
     </row>
     <row r="179" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A179" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B179" s="4">
         <v>44056</v>
@@ -16092,7 +16092,7 @@
     </row>
     <row r="180" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A180" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B180" s="4">
         <v>44056</v>
@@ -16112,7 +16112,7 @@
     </row>
     <row r="181" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A181" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B181" s="4">
         <v>44056</v>
@@ -16132,7 +16132,7 @@
     </row>
     <row r="182" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A182" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B182" s="4">
         <v>44056</v>
@@ -16152,7 +16152,7 @@
     </row>
     <row r="183" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A183" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B183" s="4">
         <v>44056</v>
@@ -16172,7 +16172,7 @@
     </row>
     <row r="184" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A184" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B184" s="4">
         <v>44056</v>
@@ -16192,7 +16192,7 @@
     </row>
     <row r="185" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A185" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B185" s="4">
         <v>44056</v>
@@ -16212,7 +16212,7 @@
     </row>
     <row r="186" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A186" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B186" s="4">
         <v>44056</v>
@@ -16232,7 +16232,7 @@
     </row>
     <row r="187" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A187" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B187" s="4">
         <v>44056</v>
@@ -16252,7 +16252,7 @@
     </row>
     <row r="188" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A188" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B188" s="4">
         <v>44056</v>
@@ -16272,7 +16272,7 @@
     </row>
     <row r="189" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A189" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B189" s="4">
         <v>44056</v>
@@ -16292,7 +16292,7 @@
     </row>
     <row r="190" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A190" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B190" s="4">
         <v>44056</v>
@@ -16312,7 +16312,7 @@
     </row>
     <row r="191" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A191" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B191" s="4">
         <v>44056</v>
@@ -16332,7 +16332,7 @@
     </row>
     <row r="192" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A192" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B192" s="4">
         <v>44056</v>
@@ -16352,7 +16352,7 @@
     </row>
     <row r="193" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A193" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B193" s="4">
         <v>44056</v>
@@ -16372,7 +16372,7 @@
     </row>
     <row r="194" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A194" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B194" s="4">
         <v>44173</v>
@@ -16392,7 +16392,7 @@
     </row>
     <row r="195" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A195" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B195" s="4">
         <v>44173</v>
@@ -16412,7 +16412,7 @@
     </row>
     <row r="196" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A196" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B196" s="4">
         <v>44173</v>
@@ -16432,7 +16432,7 @@
     </row>
     <row r="197" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A197" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B197" s="4">
         <v>44173</v>
@@ -16452,7 +16452,7 @@
     </row>
     <row r="198" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A198" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B198" s="4">
         <v>44173</v>
@@ -16472,7 +16472,7 @@
     </row>
     <row r="199" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A199" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B199" s="4">
         <v>44173</v>
@@ -16492,7 +16492,7 @@
     </row>
     <row r="200" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A200" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B200" s="4">
         <v>44173</v>
@@ -16512,7 +16512,7 @@
     </row>
     <row r="201" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A201" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B201" s="4">
         <v>44173</v>
@@ -16532,7 +16532,7 @@
     </row>
     <row r="202" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A202" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B202" s="4">
         <v>44173</v>
@@ -16552,7 +16552,7 @@
     </row>
     <row r="203" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A203" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B203" s="4">
         <v>44173</v>
@@ -16572,7 +16572,7 @@
     </row>
     <row r="204" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A204" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B204" s="4">
         <v>44173</v>
@@ -16592,7 +16592,7 @@
     </row>
     <row r="205" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A205" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B205" s="4">
         <v>44173</v>
@@ -16612,7 +16612,7 @@
     </row>
     <row r="206" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A206" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B206" s="4">
         <v>44173</v>
@@ -16632,7 +16632,7 @@
     </row>
     <row r="207" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A207" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B207" s="4">
         <v>44173</v>
@@ -16652,7 +16652,7 @@
     </row>
     <row r="208" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A208" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B208" s="4">
         <v>44173</v>
@@ -16672,7 +16672,7 @@
     </row>
     <row r="209" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A209" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B209" s="4">
         <v>44173</v>
@@ -16692,7 +16692,7 @@
     </row>
     <row r="210" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A210" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B210" s="4">
         <v>44173</v>
@@ -16712,7 +16712,7 @@
     </row>
     <row r="211" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A211" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B211" s="4">
         <v>44173</v>
@@ -16732,7 +16732,7 @@
     </row>
     <row r="212" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A212" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B212" s="4">
         <v>44173</v>
@@ -16752,7 +16752,7 @@
     </row>
     <row r="213" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A213" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B213" s="4">
         <v>44173</v>
@@ -16772,7 +16772,7 @@
     </row>
     <row r="214" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A214" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B214" s="4">
         <v>44173</v>
@@ -16792,7 +16792,7 @@
     </row>
     <row r="215" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A215" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B215" s="4">
         <v>44173</v>
@@ -16812,7 +16812,7 @@
     </row>
     <row r="216" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A216" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B216" s="4">
         <v>44173</v>
@@ -16832,7 +16832,7 @@
     </row>
     <row r="217" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A217" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B217" s="4">
         <v>44173</v>
@@ -16852,7 +16852,7 @@
     </row>
     <row r="218" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A218" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B218" s="4">
         <v>44173</v>
@@ -16872,7 +16872,7 @@
     </row>
     <row r="219" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A219" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B219" s="4">
         <v>44173</v>
@@ -16892,7 +16892,7 @@
     </row>
     <row r="220" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A220" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B220" s="4">
         <v>44173</v>
@@ -16912,7 +16912,7 @@
     </row>
     <row r="221" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A221" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B221" s="4">
         <v>44173</v>
@@ -16932,7 +16932,7 @@
     </row>
     <row r="222" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A222" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B222" s="4">
         <v>44173</v>
@@ -16952,7 +16952,7 @@
     </row>
     <row r="223" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A223" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B223" s="4">
         <v>44173</v>
@@ -16972,7 +16972,7 @@
     </row>
     <row r="224" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A224" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B224" s="4">
         <v>44173</v>
@@ -16992,7 +16992,7 @@
     </row>
     <row r="225" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A225" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B225" s="4">
         <v>44173</v>
@@ -17012,5 +17012,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>